<commit_message>
process run record coding completed.
</commit_message>
<xml_diff>
--- a/soberano/test_cases/cash_register_operation_record_test_cases.xlsx
+++ b/soberano/test_cases/cash_register_operation_record_test_cases.xlsx
@@ -49,19 +49,19 @@
     <t xml:space="preserve">mc8</t>
   </si>
   <si>
+    <t xml:space="preserve">success</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">withdrawal</t>
+  </si>
+  <si>
     <t xml:space="preserve">not enough rights</t>
   </si>
   <si>
     <t xml:space="preserve">shift manager</t>
-  </si>
-  <si>
-    <t xml:space="preserve">withdrawal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">success</t>
-  </si>
-  <si>
-    <t xml:space="preserve">checker</t>
   </si>
   <si>
     <t xml:space="preserve">accounter</t>
@@ -199,8 +199,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -288,10 +288,12 @@
         <v>0</v>
       </c>
       <c r="H3" s="0" t="n">
-        <v>0</v>
+        <f aca="false">H4-E3</f>
+        <v>50.3451</v>
       </c>
       <c r="I3" s="0" t="n">
-        <v>0</v>
+        <f aca="false">I4-F3</f>
+        <v>-1000.678</v>
       </c>
       <c r="J3" s="0" t="n">
         <v>0</v>
@@ -320,12 +322,10 @@
         <v>0</v>
       </c>
       <c r="H4" s="0" t="n">
-        <f aca="false">H3-E4</f>
-        <v>50.3451</v>
+        <v>0</v>
       </c>
       <c r="I4" s="0" t="n">
-        <f aca="false">I3-F4</f>
-        <v>-1000.678</v>
+        <v>0</v>
       </c>
       <c r="J4" s="0" t="n">
         <v>0</v>
@@ -336,7 +336,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C5" s="0" t="s">
         <v>14</v>
@@ -354,15 +354,15 @@
         <v>54321.2345</v>
       </c>
       <c r="H5" s="0" t="n">
-        <f aca="false">H4</f>
+        <f aca="false">H3</f>
         <v>50.3451</v>
       </c>
       <c r="I5" s="0" t="n">
-        <f aca="false">I4</f>
+        <f aca="false">I3</f>
         <v>-1000.678</v>
       </c>
       <c r="J5" s="0" t="n">
-        <f aca="false">J4</f>
+        <f aca="false">J3</f>
         <v>0</v>
       </c>
     </row>
@@ -371,10 +371,10 @@
         <v>4</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D6" s="0" t="s">
         <v>15</v>
@@ -406,7 +406,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C7" s="0" t="s">
         <v>16</v>
@@ -441,10 +441,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" s="0" t="s">
         <v>11</v>
@@ -476,10 +476,10 @@
         <v>7</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>15</v>
@@ -511,10 +511,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>15</v>
@@ -546,10 +546,10 @@
         <v>9</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>11</v>
@@ -581,10 +581,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>15</v>
@@ -616,7 +616,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>14</v>
@@ -651,10 +651,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D14" s="0" t="s">
         <v>11</v>
@@ -686,7 +686,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>16</v>
@@ -721,10 +721,10 @@
         <v>14</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>15</v>
@@ -756,10 +756,10 @@
         <v>15</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>11</v>
@@ -791,10 +791,10 @@
         <v>16</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>11</v>
@@ -826,10 +826,10 @@
         <v>17</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>15</v>
@@ -861,10 +861,10 @@
         <v>18</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>15</v>
@@ -904,10 +904,10 @@
         <v>20</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D22" s="0" t="s">
         <v>18</v>
@@ -939,10 +939,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D23" s="0" t="s">
         <v>18</v>
@@ -974,7 +974,7 @@
         <v>22</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>14</v>
@@ -1017,7 +1017,7 @@
         <v>24</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>19</v>
@@ -1060,10 +1060,10 @@
         <v>26</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D28" s="0" t="s">
         <v>18</v>

</xml_diff>